<commit_message>
Olga updated best cluster identification method keeping inly PERMANOVA and Shannon
</commit_message>
<xml_diff>
--- a/singleM_genes/Results/best_cluster.xlsx
+++ b/singleM_genes/Results/best_cluster.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t xml:space="preserve">cluster</t>
   </si>
@@ -65,27 +65,126 @@
     <t xml:space="preserve">sum_F</t>
   </si>
   <si>
+    <t xml:space="preserve">57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ureA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ureB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ureC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ureD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ureE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ureF</t>
+  </si>
+  <si>
     <t xml:space="preserve">73</t>
   </si>
   <si>
+    <t xml:space="preserve">ureG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ureJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70</t>
+  </si>
+  <si>
     <t xml:space="preserve">anfH</t>
   </si>
   <si>
+    <t xml:space="preserve">76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nifH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vnfH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">narB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">narC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nasA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nasB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nirA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nirB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nirD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asnB</t>
+  </si>
+  <si>
     <t xml:space="preserve">67</t>
   </si>
   <si>
-    <t xml:space="preserve">asnB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86</t>
-  </si>
-  <si>
     <t xml:space="preserve">gdhA</t>
   </si>
   <si>
-    <t xml:space="preserve">51</t>
-  </si>
-  <si>
     <t xml:space="preserve">glnA</t>
   </si>
   <si>
@@ -95,205 +194,85 @@
     <t xml:space="preserve">glsA</t>
   </si>
   <si>
-    <t xml:space="preserve">96</t>
+    <t xml:space="preserve">80</t>
   </si>
   <si>
     <t xml:space="preserve">gltB</t>
   </si>
   <si>
-    <t xml:space="preserve">70</t>
-  </si>
-  <si>
     <t xml:space="preserve">gltD</t>
   </si>
   <si>
+    <t xml:space="preserve">81</t>
+  </si>
+  <si>
     <t xml:space="preserve">gltS</t>
   </si>
   <si>
-    <t xml:space="preserve">72</t>
+    <t xml:space="preserve">62</t>
   </si>
   <si>
     <t xml:space="preserve">gudB</t>
   </si>
   <si>
-    <t xml:space="preserve">79</t>
+    <t xml:space="preserve">napA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">narG_nxrA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">narH_nxrB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">narI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">narJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nrfA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nrfB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nrfC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nrfD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nrfH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nirK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">norB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">norC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nosZ</t>
   </si>
   <si>
     <t xml:space="preserve">hzsA</t>
   </si>
   <si>
-    <t xml:space="preserve">71</t>
-  </si>
-  <si>
     <t xml:space="preserve">hzsB</t>
   </si>
   <si>
-    <t xml:space="preserve">74</t>
-  </si>
-  <si>
     <t xml:space="preserve">hzsC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">napA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">narB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">narC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">narG_nxrA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">narH_nxrB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93</t>
-  </si>
-  <si>
-    <t xml:space="preserve">narI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">92</t>
-  </si>
-  <si>
-    <t xml:space="preserve">narJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nasA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nasB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nifH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nirA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nirB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">97</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nirD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nirK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77</t>
-  </si>
-  <si>
-    <t xml:space="preserve">norB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">norC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nosZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nrfA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nrfB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nrfC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nrfD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nrfH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ureA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ureB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ureC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ureD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ureE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ureF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ureG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ureJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vnfH</t>
   </si>
 </sst>
 </file>
@@ -686,49 +665,49 @@
         <v>18</v>
       </c>
       <c r="C2" t="n">
-        <v>0.158761726233372</v>
+        <v>0.251799703520217</v>
       </c>
       <c r="D2" t="n">
-        <v>22.0806905113041</v>
+        <v>33.6540502195618</v>
       </c>
       <c r="E2" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F2" t="n">
-        <v>25</v>
+        <v>1844</v>
       </c>
       <c r="G2" t="n">
-        <v>415.557932077092</v>
+        <v>11.9005970196835</v>
       </c>
       <c r="H2" t="n">
-        <v>0.000000000000000000000000000000000000000260721541042991</v>
+        <v>0.000823047902966335</v>
       </c>
       <c r="I2" t="n">
-        <v>0.780305591274034</v>
+        <v>0.106349718738231</v>
       </c>
       <c r="J2" t="n">
-        <v>332.908022388903</v>
+        <v>46.2472977378663</v>
       </c>
       <c r="K2" t="n">
-        <v>0.00000000000000000000000000000000000515441897443602</v>
+        <v>0.000000000772130480951935</v>
       </c>
       <c r="L2" t="n">
-        <v>0.739946846515965</v>
+        <v>0.316226682155591</v>
       </c>
       <c r="M2" t="n">
-        <v>96.944711079893</v>
+        <v>0.0139133223324005</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0000000000000000502041740160142</v>
+        <v>0.90634011701706</v>
       </c>
       <c r="O2" t="n">
-        <v>0.453129738943119</v>
+        <v>0.000139113867963143</v>
       </c>
       <c r="P2" t="n">
-        <v>2.13214390296649</v>
+        <v>0.819826089196025</v>
       </c>
       <c r="Q2" t="n">
-        <v>867.491356057192</v>
+        <v>113.55539817699</v>
       </c>
     </row>
     <row r="3">
@@ -739,49 +718,49 @@
         <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>0.139845144125707</v>
+        <v>0.0999810246879966</v>
       </c>
       <c r="D3" t="n">
-        <v>19.0220188271529</v>
+        <v>11.5531192705654</v>
       </c>
       <c r="E3" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F3" t="n">
-        <v>70</v>
+        <v>1925</v>
       </c>
       <c r="G3" t="n">
-        <v>324.102676357025</v>
+        <v>181.40387619477</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0000000000000000000000000000000000164376892775679</v>
+        <v>0.00000000000000000000000154984411085112</v>
       </c>
       <c r="I3" t="n">
-        <v>0.734755633390669</v>
+        <v>0.635604108162054</v>
       </c>
       <c r="J3" t="n">
-        <v>262.06534265358</v>
+        <v>173.741652255615</v>
       </c>
       <c r="K3" t="n">
-        <v>0.000000000000000000000000000000120103605777324</v>
+        <v>0.0000000000000000000000064302717888422</v>
       </c>
       <c r="L3" t="n">
-        <v>0.691346090410265</v>
+        <v>0.625551302242973</v>
       </c>
       <c r="M3" t="n">
-        <v>225.859574623025</v>
+        <v>32.9003492601425</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0000000000000000000000000000436774919106448</v>
+        <v>0.0000000960636893448596</v>
       </c>
       <c r="O3" t="n">
-        <v>0.658752420349813</v>
+        <v>0.240323340575444</v>
       </c>
       <c r="P3" t="n">
-        <v>2.22469928827645</v>
+        <v>0.825513351618966</v>
       </c>
       <c r="Q3" t="n">
-        <v>831.049612460783</v>
+        <v>196.847890796746</v>
       </c>
     </row>
     <row r="4">
@@ -792,49 +771,49 @@
         <v>22</v>
       </c>
       <c r="C4" t="n">
-        <v>0.175900254464343</v>
+        <v>0.0848778286501301</v>
       </c>
       <c r="D4" t="n">
-        <v>24.9731053598993</v>
+        <v>10.8517816123029</v>
       </c>
       <c r="E4" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F4" t="n">
-        <v>140</v>
+        <v>1978</v>
       </c>
       <c r="G4" t="n">
-        <v>439.817080057324</v>
+        <v>197.999251818081</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0000000000000000000000000000000000000000191365051954315</v>
+        <v>0.0000000000000000000000000063588283082778</v>
       </c>
       <c r="I4" t="n">
-        <v>0.789877135256061</v>
+        <v>0.628570546359361</v>
       </c>
       <c r="J4" t="n">
-        <v>381.896492486931</v>
+        <v>186.359716136638</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0000000000000000000000000000000000000119978100000826</v>
+        <v>0.0000000000000000000000000581828480627772</v>
       </c>
       <c r="L4" t="n">
-        <v>0.765482416168591</v>
+        <v>0.614319259359733</v>
       </c>
       <c r="M4" t="n">
-        <v>106.677621211532</v>
+        <v>90.1797472426351</v>
       </c>
       <c r="N4" t="n">
-        <v>0.00000000000000000362854365535082</v>
+        <v>0.000000000000000335335612096496</v>
       </c>
       <c r="O4" t="n">
-        <v>0.476925767690666</v>
+        <v>0.435272986104296</v>
       </c>
       <c r="P4" t="n">
-        <v>2.20818557357966</v>
+        <v>0.784074916659993</v>
       </c>
       <c r="Q4" t="n">
-        <v>953.364299115686</v>
+        <v>208.063279361244</v>
       </c>
     </row>
     <row r="5">
@@ -845,49 +824,49 @@
         <v>24</v>
       </c>
       <c r="C5" t="n">
-        <v>0.563278383777349</v>
+        <v>0.13987803233348</v>
       </c>
       <c r="D5" t="n">
-        <v>150.905218459236</v>
+        <v>15.9373294532523</v>
       </c>
       <c r="E5" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F5" t="n">
-        <v>156</v>
+        <v>2000</v>
       </c>
       <c r="G5" t="n">
-        <v>46.9499952733394</v>
+        <v>119.879186780643</v>
       </c>
       <c r="H5" t="n">
-        <v>0.000000000361446274180731</v>
+        <v>0.00000000000000000106900378738976</v>
       </c>
       <c r="I5" t="n">
-        <v>0.28636777448553</v>
+        <v>0.550209446583511</v>
       </c>
       <c r="J5" t="n">
-        <v>305.545214177662</v>
+        <v>115.945479786196</v>
       </c>
       <c r="K5" t="n">
-        <v>0.000000000000000000000000000000000204749496689107</v>
+        <v>0.00000000000000000262948665810407</v>
       </c>
       <c r="L5" t="n">
-        <v>0.723106555051865</v>
+        <v>0.541939375873073</v>
       </c>
       <c r="M5" t="n">
-        <v>21.5875299964547</v>
+        <v>32.8202241938052</v>
       </c>
       <c r="N5" t="n">
-        <v>0.00000892785127956958</v>
+        <v>0.000000111265244364946</v>
       </c>
       <c r="O5" t="n">
-        <v>0.155768199325054</v>
+        <v>0.250880354288212</v>
       </c>
       <c r="P5" t="n">
-        <v>1.7285209126398</v>
+        <v>0.821695440540033</v>
       </c>
       <c r="Q5" t="n">
-        <v>524.987957906692</v>
+        <v>147.820138692701</v>
       </c>
     </row>
     <row r="6">
@@ -898,49 +877,49 @@
         <v>26</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0290867179488445</v>
+        <v>0.447543170127667</v>
       </c>
       <c r="D6" t="n">
-        <v>2.51648046521852</v>
+        <v>66.4278871508374</v>
       </c>
       <c r="E6" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F6" t="n">
-        <v>255</v>
+        <v>2042</v>
       </c>
       <c r="G6" t="n">
-        <v>92.8174314755556</v>
+        <v>34.9604087265415</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00000000000000314538476275146</v>
+        <v>0.0000000743565283763557</v>
       </c>
       <c r="I6" t="n">
-        <v>0.524933716664623</v>
+        <v>0.298908058779791</v>
       </c>
       <c r="J6" t="n">
-        <v>84.3080072826521</v>
+        <v>114.743528614679</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0000000000000255304414025075</v>
+        <v>0.0000000000000000297593319801365</v>
       </c>
       <c r="L6" t="n">
-        <v>0.500915010781795</v>
+        <v>0.583213737308756</v>
       </c>
       <c r="M6" t="n">
-        <v>61.8059092309326</v>
+        <v>7.70186387762169</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0000000000114666857531666</v>
+        <v>0.00683085361118013</v>
       </c>
       <c r="O6" t="n">
-        <v>0.423891662257956</v>
+        <v>0.0858606894515501</v>
       </c>
       <c r="P6" t="n">
-        <v>1.47882710765322</v>
+        <v>1.47830007756409</v>
       </c>
       <c r="Q6" t="n">
-        <v>241.447828454359</v>
+        <v>247.599302916354</v>
       </c>
     </row>
     <row r="7">
@@ -951,49 +930,49 @@
         <v>28</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0652337084360722</v>
+        <v>0.14022220989572</v>
       </c>
       <c r="D7" t="n">
-        <v>8.16497551944349</v>
+        <v>15.4936660302399</v>
       </c>
       <c r="E7" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F7" t="n">
-        <v>303</v>
+        <v>2117</v>
       </c>
       <c r="G7" t="n">
-        <v>154.061089929283</v>
+        <v>75.7777339054899</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0000000000000000000000437844217150531</v>
+        <v>0.0000000000000964542313722323</v>
       </c>
       <c r="I7" t="n">
-        <v>0.568362984039782</v>
+        <v>0.443721392552415</v>
       </c>
       <c r="J7" t="n">
-        <v>103.844661326562</v>
+        <v>99.0504700275797</v>
       </c>
       <c r="K7" t="n">
-        <v>0.00000000000000000770085558052521</v>
+        <v>0.000000000000000208781682230503</v>
       </c>
       <c r="L7" t="n">
-        <v>0.470215855356394</v>
+        <v>0.510436640599232</v>
       </c>
       <c r="M7" t="n">
-        <v>80.3186494751762</v>
+        <v>3.34752009084237</v>
       </c>
       <c r="N7" t="n">
-        <v>0.00000000000000600435966089806</v>
+        <v>0.0704427963385904</v>
       </c>
       <c r="O7" t="n">
-        <v>0.407050472364402</v>
+        <v>0.0340376665090315</v>
       </c>
       <c r="P7" t="n">
-        <v>1.51086302019665</v>
+        <v>0.790881060390672</v>
       </c>
       <c r="Q7" t="n">
-        <v>346.389376250465</v>
+        <v>130.037802088059</v>
       </c>
     </row>
     <row r="8">
@@ -1004,261 +983,261 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>0.135876892629955</v>
+        <v>0.159110037293536</v>
       </c>
       <c r="D8" t="n">
-        <v>18.3973745200369</v>
+        <v>21.949083880899</v>
       </c>
       <c r="E8" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F8" t="n">
-        <v>328</v>
+        <v>2166</v>
       </c>
       <c r="G8" t="n">
-        <v>359.174551459128</v>
+        <v>108.122950427226</v>
       </c>
       <c r="H8" t="n">
-        <v>0.000000000000000000000000000000000000184722511088021</v>
+        <v>0.00000000000000000271363401444318</v>
       </c>
       <c r="I8" t="n">
-        <v>0.754291783041576</v>
+        <v>0.482426945661391</v>
       </c>
       <c r="J8" t="n">
-        <v>338.607048049756</v>
+        <v>103.336821951424</v>
       </c>
       <c r="K8" t="n">
-        <v>0.00000000000000000000000000000000000246289973565362</v>
+        <v>0.00000000000000000959970128704164</v>
       </c>
       <c r="L8" t="n">
-        <v>0.743199758430378</v>
+        <v>0.471133031982699</v>
       </c>
       <c r="M8" t="n">
-        <v>204.157716488732</v>
+        <v>49.3597993243517</v>
       </c>
       <c r="N8" t="n">
-        <v>0.00000000000000000000000000203740259293917</v>
+        <v>0.000000000155835972380825</v>
       </c>
       <c r="O8" t="n">
-        <v>0.63569301314264</v>
+        <v>0.298499390577591</v>
       </c>
       <c r="P8" t="n">
-        <v>2.26906144724455</v>
+        <v>0.789353106569771</v>
       </c>
       <c r="Q8" t="n">
-        <v>920.336690517653</v>
+        <v>147.234989713222</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0826191710421151</v>
+        <v>0.0839839846340051</v>
       </c>
       <c r="D9" t="n">
-        <v>10.5370013268189</v>
+        <v>7.33471757918549</v>
       </c>
       <c r="E9" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F9" t="n">
-        <v>394</v>
+        <v>2228</v>
       </c>
       <c r="G9" t="n">
-        <v>158.679059449303</v>
+        <v>64.4977445561782</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0000000000000000000000161980181683272</v>
+        <v>0.00000000000703087640081264</v>
       </c>
       <c r="I9" t="n">
-        <v>0.575593444660907</v>
+        <v>0.446358140428293</v>
       </c>
       <c r="J9" t="n">
-        <v>148.668563725883</v>
+        <v>79.5588901570176</v>
       </c>
       <c r="K9" t="n">
-        <v>0.000000000000000000000142930784791708</v>
+        <v>0.00000000000012639730636266</v>
       </c>
       <c r="L9" t="n">
-        <v>0.559601639128366</v>
+        <v>0.498617720884909</v>
       </c>
       <c r="M9" t="n">
-        <v>19.0813545809846</v>
+        <v>5.72737754473326</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0000272328661201795</v>
+        <v>0.0190449557579853</v>
       </c>
       <c r="O9" t="n">
-        <v>0.140220198716709</v>
+        <v>0.0668092003834442</v>
       </c>
       <c r="P9" t="n">
-        <v>1.3580344535481</v>
+        <v>0.666585690152919</v>
       </c>
       <c r="Q9" t="n">
-        <v>336.96597908299</v>
+        <v>94.2283253153886</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" t="n">
-        <v>0.317699155977275</v>
+        <v>0.189745660546746</v>
       </c>
       <c r="D10" t="n">
-        <v>54.4786095092434</v>
+        <v>27.3991032235009</v>
       </c>
       <c r="E10" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F10" t="n">
-        <v>431</v>
+        <v>22</v>
       </c>
       <c r="G10" t="n">
-        <v>488.182743515419</v>
+        <v>287.314938621333</v>
       </c>
       <c r="H10" t="n">
-        <v>0.000000000000000000000000000000000000000000144947722773459</v>
+        <v>0.00000000000000000000000000000000272515604940217</v>
       </c>
       <c r="I10" t="n">
-        <v>0.806669966627991</v>
+        <v>0.710621624818127</v>
       </c>
       <c r="J10" t="n">
-        <v>485.582266301905</v>
+        <v>277.829302847624</v>
       </c>
       <c r="K10" t="n">
-        <v>0.00000000000000000000000000000000000000000018656816733725</v>
+        <v>0.0000000000000000000000000000000109808356927117</v>
       </c>
       <c r="L10" t="n">
-        <v>0.805835640139166</v>
+        <v>0.703669410663895</v>
       </c>
       <c r="M10" t="n">
-        <v>83.6041054556771</v>
+        <v>56.0188749446415</v>
       </c>
       <c r="N10" t="n">
-        <v>0.00000000000000225944145008037</v>
+        <v>0.0000000000146178591926739</v>
       </c>
       <c r="O10" t="n">
-        <v>0.416761687233511</v>
+        <v>0.323773200828899</v>
       </c>
       <c r="P10" t="n">
-        <v>2.34696644997794</v>
+        <v>1.08316073175739</v>
       </c>
       <c r="Q10" t="n">
-        <v>1111.84772478224</v>
+        <v>332.627509294626</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" t="n">
-        <v>0.122530787976106</v>
+        <v>0.152884324340732</v>
       </c>
       <c r="D11" t="n">
-        <v>16.0587293823688</v>
+        <v>21.1157300730442</v>
       </c>
       <c r="E11" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F11" t="n">
-        <v>489</v>
+        <v>1098</v>
       </c>
       <c r="G11" t="n">
-        <v>206.052433791313</v>
+        <v>325.96697235705</v>
       </c>
       <c r="H11" t="n">
-        <v>0.00000000000000000000000000212278448609161</v>
+        <v>0.0000000000000000000000000000000000128341406485798</v>
       </c>
       <c r="I11" t="n">
-        <v>0.641803058017773</v>
+        <v>0.735871955921596</v>
       </c>
       <c r="J11" t="n">
-        <v>158.826063925989</v>
+        <v>307.128793173837</v>
       </c>
       <c r="K11" t="n">
-        <v>0.000000000000000000000020970134973502</v>
+        <v>0.000000000000000000000000000000000164392642948717</v>
       </c>
       <c r="L11" t="n">
-        <v>0.580025369567878</v>
+        <v>0.724140398192572</v>
       </c>
       <c r="M11" t="n">
-        <v>84.5017452917237</v>
+        <v>77.7864167388719</v>
       </c>
       <c r="N11" t="n">
-        <v>0.00000000000000197452702464375</v>
+        <v>0.000000000000012900563441117</v>
       </c>
       <c r="O11" t="n">
-        <v>0.423563940095662</v>
+        <v>0.399342100138078</v>
       </c>
       <c r="P11" t="n">
-        <v>1.76792315565742</v>
+        <v>1.02990904687404</v>
       </c>
       <c r="Q11" t="n">
-        <v>465.438972391394</v>
+        <v>349.360253319925</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
       </c>
       <c r="C12" t="n">
-        <v>0.166697193884479</v>
+        <v>0.518951361652242</v>
       </c>
       <c r="D12" t="n">
-        <v>22.0048356884456</v>
+        <v>126.218649161665</v>
       </c>
       <c r="E12" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F12" t="n">
-        <v>532</v>
+        <v>2246</v>
       </c>
       <c r="G12" t="n">
-        <v>222.749812060029</v>
+        <v>48.4861263103213</v>
       </c>
       <c r="H12" t="n">
-        <v>0.000000000000000000000000000335451660232891</v>
+        <v>0.000000000207207230144478</v>
       </c>
       <c r="I12" t="n">
-        <v>0.669421300889704</v>
+        <v>0.292992091792635</v>
       </c>
       <c r="J12" t="n">
-        <v>142.328652848628</v>
+        <v>171.154937604359</v>
       </c>
       <c r="K12" t="n">
-        <v>0.00000000000000000000147938893528569</v>
+        <v>0.00000000000000000000000119763630064749</v>
       </c>
       <c r="L12" t="n">
-        <v>0.564060606046238</v>
+        <v>0.593968435964673</v>
       </c>
       <c r="M12" t="n">
-        <v>54.0829583182171</v>
+        <v>16.5838587394451</v>
       </c>
       <c r="N12" t="n">
-        <v>0.0000000000364587199012767</v>
+        <v>0.0000850047601984521</v>
       </c>
       <c r="O12" t="n">
-        <v>0.329607406354354</v>
+        <v>0.124145678197483</v>
       </c>
       <c r="P12" t="n">
-        <v>1.72978650717477</v>
+        <v>1.63187115926916</v>
       </c>
       <c r="Q12" t="n">
-        <v>441.16625891532</v>
+        <v>423.592235927689</v>
       </c>
     </row>
     <row r="13">
@@ -1269,49 +1248,49 @@
         <v>39</v>
       </c>
       <c r="C13" t="n">
-        <v>0.082738386327401</v>
+        <v>0.442244738265432</v>
       </c>
       <c r="D13" t="n">
-        <v>10.5535771431085</v>
+        <v>88.8049187231158</v>
       </c>
       <c r="E13" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F13" t="n">
-        <v>586</v>
+        <v>1351</v>
       </c>
       <c r="G13" t="n">
-        <v>196.701876575762</v>
+        <v>83.3558098539466</v>
       </c>
       <c r="H13" t="n">
-        <v>0.00000000000000000000000000810494846623105</v>
+        <v>0.00000000000000335940914423154</v>
       </c>
       <c r="I13" t="n">
-        <v>0.627034427472596</v>
+        <v>0.426687130094906</v>
       </c>
       <c r="J13" t="n">
-        <v>184.679848910188</v>
+        <v>110.272033479969</v>
       </c>
       <c r="K13" t="n">
-        <v>0.00000000000000000000000008065181583648</v>
+        <v>0.00000000000000000226695189760447</v>
       </c>
       <c r="L13" t="n">
-        <v>0.612171643473506</v>
+        <v>0.496112946615511</v>
       </c>
       <c r="M13" t="n">
-        <v>96.7005810640409</v>
+        <v>25.0892629744119</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0000000000000000537076490495902</v>
+        <v>0.00000205834316407782</v>
       </c>
       <c r="O13" t="n">
-        <v>0.452504998267001</v>
+        <v>0.18301406273586</v>
       </c>
       <c r="P13" t="n">
-        <v>1.7744494555405</v>
+        <v>1.38060242314637</v>
       </c>
       <c r="Q13" t="n">
-        <v>488.635883693099</v>
+        <v>287.881870926201</v>
       </c>
     </row>
     <row r="14">
@@ -1322,49 +1301,49 @@
         <v>41</v>
       </c>
       <c r="C14" t="n">
-        <v>0.195523396781381</v>
+        <v>0.1992160982371</v>
       </c>
       <c r="D14" t="n">
-        <v>28.4361749389558</v>
+        <v>29.1068332448095</v>
       </c>
       <c r="E14" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F14" t="n">
-        <v>629</v>
+        <v>672</v>
       </c>
       <c r="G14" t="n">
-        <v>270.177786181858</v>
+        <v>181.801765558683</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0000000000000000000000000000000346414142633809</v>
+        <v>0.000000000000000000000000141726627086579</v>
       </c>
       <c r="I14" t="n">
-        <v>0.697813241937788</v>
+        <v>0.608436048624948</v>
       </c>
       <c r="J14" t="n">
-        <v>296.696186398834</v>
+        <v>277.85275984512</v>
       </c>
       <c r="K14" t="n">
-        <v>0.000000000000000000000000000000000709055810592888</v>
+        <v>0.0000000000000000000000000000000109426053649268</v>
       </c>
       <c r="L14" t="n">
-        <v>0.717183759854137</v>
+        <v>0.703687014759899</v>
       </c>
       <c r="M14" t="n">
-        <v>67.2293462682835</v>
+        <v>30.5142976076208</v>
       </c>
       <c r="N14" t="n">
-        <v>0.000000000000350803113704278</v>
+        <v>0.000000203298016397081</v>
       </c>
       <c r="O14" t="n">
-        <v>0.364922025888215</v>
+        <v>0.206856542738569</v>
       </c>
       <c r="P14" t="n">
-        <v>1.97544242446152</v>
+        <v>1.1021192112341</v>
       </c>
       <c r="Q14" t="n">
-        <v>662.539493787931</v>
+        <v>336.066426334739</v>
       </c>
     </row>
     <row r="15">
@@ -1375,526 +1354,526 @@
         <v>43</v>
       </c>
       <c r="C15" t="n">
-        <v>0.107313244305598</v>
+        <v>0.415512932488</v>
       </c>
       <c r="D15" t="n">
-        <v>14.0650116109185</v>
+        <v>83.1755154276325</v>
       </c>
       <c r="E15" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F15" t="n">
-        <v>695</v>
+        <v>733</v>
       </c>
       <c r="G15" t="n">
-        <v>243.453997840871</v>
+        <v>111.294270444673</v>
       </c>
       <c r="H15" t="n">
-        <v>0.00000000000000000000000000000230970033111841</v>
+        <v>0.0000000000000000010866460273546</v>
       </c>
       <c r="I15" t="n">
-        <v>0.675409342937426</v>
+        <v>0.487503563834053</v>
       </c>
       <c r="J15" t="n">
-        <v>210.223715006393</v>
+        <v>181.818544549091</v>
       </c>
       <c r="K15" t="n">
-        <v>0.000000000000000000000000000678337982371438</v>
+        <v>0.00000000000000000000000014125934505063</v>
       </c>
       <c r="L15" t="n">
-        <v>0.642446452887089</v>
+        <v>0.608458035372103</v>
       </c>
       <c r="M15" t="n">
-        <v>138.192696312083</v>
+        <v>33.0177325795099</v>
       </c>
       <c r="N15" t="n">
-        <v>0.00000000000000000000152810729032627</v>
+        <v>0.0000000737984390302094</v>
       </c>
       <c r="O15" t="n">
-        <v>0.541522928787441</v>
+        <v>0.220092198514002</v>
       </c>
       <c r="P15" t="n">
-        <v>1.96669196891755</v>
+        <v>1.4394839003481</v>
       </c>
       <c r="Q15" t="n">
-        <v>605.935420770265</v>
+        <v>348.169575404356</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
       <c r="C16" t="n">
-        <v>0.415512932488</v>
+        <v>0.310908276236362</v>
       </c>
       <c r="D16" t="n">
-        <v>83.1755154276325</v>
+        <v>52.7887174743251</v>
       </c>
       <c r="E16" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F16" t="n">
-        <v>733</v>
+        <v>971</v>
       </c>
       <c r="G16" t="n">
-        <v>111.294270444673</v>
+        <v>148.903469859413</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0000000000000000010866460273546</v>
+        <v>0.000000000000000000000135682801070069</v>
       </c>
       <c r="I16" t="n">
-        <v>0.487503563834053</v>
+        <v>0.559990698647672</v>
       </c>
       <c r="J16" t="n">
-        <v>181.818544549091</v>
+        <v>222.902222243192</v>
       </c>
       <c r="K16" t="n">
-        <v>0.00000000000000000000000014125934505063</v>
+        <v>0.0000000000000000000000000000726619938820393</v>
       </c>
       <c r="L16" t="n">
-        <v>0.608458035372103</v>
+        <v>0.655783362556867</v>
       </c>
       <c r="M16" t="n">
-        <v>33.0177325795099</v>
+        <v>14.6955059906908</v>
       </c>
       <c r="N16" t="n">
-        <v>0.0000000737984390302094</v>
+        <v>0.000204985696993699</v>
       </c>
       <c r="O16" t="n">
-        <v>0.220092198514002</v>
+        <v>0.111586996687112</v>
       </c>
       <c r="P16" t="n">
-        <v>1.73156673020816</v>
+        <v>1.27759991502959</v>
       </c>
       <c r="Q16" t="n">
-        <v>409.306063000906</v>
+        <v>328.479657191842</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C17" t="n">
-        <v>0.196635714582472</v>
+        <v>0.176949716619007</v>
       </c>
       <c r="D17" t="n">
-        <v>28.3927768580251</v>
+        <v>25.1541336689393</v>
       </c>
       <c r="E17" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F17" t="n">
-        <v>794</v>
+        <v>1031</v>
       </c>
       <c r="G17" t="n">
-        <v>318.386218303389</v>
+        <v>140.752121535744</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0000000000000000000000000000000000474961301609715</v>
+        <v>0.000000000000000000000848888772219523</v>
       </c>
       <c r="I17" t="n">
-        <v>0.732956537035017</v>
+        <v>0.546075511220283</v>
       </c>
       <c r="J17" t="n">
-        <v>244.786816561112</v>
+        <v>226.087154535332</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0000000000000000000000000000023404764058379</v>
+        <v>0.000000000000000000000000000042007482449489</v>
       </c>
       <c r="L17" t="n">
-        <v>0.678480491317089</v>
+        <v>0.658978780017393</v>
       </c>
       <c r="M17" t="n">
-        <v>148.71004722508</v>
+        <v>49.3665199347513</v>
       </c>
       <c r="N17" t="n">
-        <v>0.000000000000000000000161824038681303</v>
+        <v>0.000000000151004200915381</v>
       </c>
       <c r="O17" t="n">
-        <v>0.56178467264083</v>
+        <v>0.296733501152232</v>
       </c>
       <c r="P17" t="n">
-        <v>2.16985741557541</v>
+        <v>1.01287821325541</v>
       </c>
       <c r="Q17" t="n">
-        <v>740.275858947606</v>
+        <v>276.395421873211</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" t="n">
-        <v>0.287300856953506</v>
+        <v>0.451342143485784</v>
       </c>
       <c r="D18" t="n">
-        <v>47.1646424603141</v>
+        <v>96.2476526324354</v>
       </c>
       <c r="E18" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F18" t="n">
-        <v>834</v>
+        <v>1534</v>
       </c>
       <c r="G18" t="n">
-        <v>281.525966115116</v>
+        <v>92.1137075825553</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0000000000000000000000000000000063539639534534</v>
+        <v>0.000000000000000193608664933184</v>
       </c>
       <c r="I18" t="n">
-        <v>0.706418125924061</v>
+        <v>0.440495788857792</v>
       </c>
       <c r="J18" t="n">
-        <v>289.863955079896</v>
+        <v>125.53522511999</v>
       </c>
       <c r="K18" t="n">
-        <v>0.00000000000000000000000000000000188442723151264</v>
+        <v>0.0000000000000000000306288784628767</v>
       </c>
       <c r="L18" t="n">
-        <v>0.712434590139535</v>
+        <v>0.517595846367816</v>
       </c>
       <c r="M18" t="n">
-        <v>37.2986400883131</v>
+        <v>12.5056256446736</v>
       </c>
       <c r="N18" t="n">
-        <v>0.0000000136193446296277</v>
+        <v>0.00058247739223693</v>
       </c>
       <c r="O18" t="n">
-        <v>0.241730193260065</v>
+        <v>0.0965643429188593</v>
       </c>
       <c r="P18" t="n">
-        <v>1.94788376627717</v>
+        <v>1.42028013333938</v>
       </c>
       <c r="Q18" t="n">
-        <v>655.853203743639</v>
+        <v>318.030530384861</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C19" t="n">
-        <v>0.120493458734045</v>
+        <v>0.0878086401094586</v>
       </c>
       <c r="D19" t="n">
-        <v>13.2891171910774</v>
+        <v>11.2625610639849</v>
       </c>
       <c r="E19" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F19" t="n">
-        <v>911</v>
+        <v>1160</v>
       </c>
       <c r="G19" t="n">
-        <v>95.1986777561984</v>
+        <v>142.526201886027</v>
       </c>
       <c r="H19" t="n">
-        <v>0.000000000000000448917890198369</v>
+        <v>0.000000000000000000000566744909438912</v>
       </c>
       <c r="I19" t="n">
-        <v>0.495313905733299</v>
+        <v>0.549178467724113</v>
       </c>
       <c r="J19" t="n">
-        <v>105.409570385691</v>
+        <v>135.479497336555</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0000000000000000355946624822933</v>
+        <v>0.0000000000000000000028684215347453</v>
       </c>
       <c r="L19" t="n">
-        <v>0.520773648127573</v>
+        <v>0.536596035582091</v>
       </c>
       <c r="M19" t="n">
-        <v>16.9121379444279</v>
+        <v>25.2912513623787</v>
       </c>
       <c r="N19" t="n">
-        <v>0.0000820516278544242</v>
+        <v>0.00000179662999924647</v>
       </c>
       <c r="O19" t="n">
-        <v>0.14846651331115</v>
+        <v>0.177742841673157</v>
       </c>
       <c r="P19" t="n">
-        <v>1.28504752590607</v>
+        <v>0.712213315801008</v>
       </c>
       <c r="Q19" t="n">
-        <v>230.809503277395</v>
+        <v>158.004619464525</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" t="n">
-        <v>0.122320236556204</v>
+        <v>0.0998939627108523</v>
       </c>
       <c r="D20" t="n">
-        <v>11.9856248052906</v>
+        <v>12.9846853070437</v>
       </c>
       <c r="E20" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F20" t="n">
-        <v>961</v>
+        <v>1196</v>
       </c>
       <c r="G20" t="n">
-        <v>63.9600568770116</v>
+        <v>104.258498881091</v>
       </c>
       <c r="H20" t="n">
-        <v>0.00000000000535228658209994</v>
+        <v>0.0000000000000000068949904518616</v>
       </c>
       <c r="I20" t="n">
-        <v>0.426513954509019</v>
+        <v>0.471206753224525</v>
       </c>
       <c r="J20" t="n">
-        <v>85.8619014724759</v>
+        <v>109.08798613559</v>
       </c>
       <c r="K20" t="n">
-        <v>0.0000000000000141258630920512</v>
+        <v>0.00000000000000000192742807185313</v>
       </c>
       <c r="L20" t="n">
-        <v>0.499598228210148</v>
+        <v>0.482502356715973</v>
       </c>
       <c r="M20" t="n">
-        <v>6.28598685547982</v>
+        <v>26.4452707565038</v>
       </c>
       <c r="N20" t="n">
-        <v>0.0140495307807824</v>
+        <v>0.00000110136484626137</v>
       </c>
       <c r="O20" t="n">
-        <v>0.0681142074725136</v>
+        <v>0.184357913070514</v>
       </c>
       <c r="P20" t="n">
-        <v>1.11654662674788</v>
+        <v>0.682290282137678</v>
       </c>
       <c r="Q20" t="n">
-        <v>168.093570010258</v>
+        <v>135.057356749677</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C21" t="n">
-        <v>0.132808677093866</v>
+        <v>0.127452820623112</v>
       </c>
       <c r="D21" t="n">
-        <v>17.9183241454829</v>
+        <v>11.5395167931392</v>
       </c>
       <c r="E21" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F21" t="n">
-        <v>995</v>
+        <v>1239</v>
       </c>
       <c r="G21" t="n">
-        <v>345.196536281048</v>
+        <v>48.6673465758183</v>
       </c>
       <c r="H21" t="n">
-        <v>0.00000000000000000000000000000000000106067564271651</v>
+        <v>0.000000000829802823473975</v>
       </c>
       <c r="I21" t="n">
-        <v>0.746860932923877</v>
+        <v>0.381204339881193</v>
       </c>
       <c r="J21" t="n">
-        <v>280.347193346012</v>
+        <v>61.2923233145498</v>
       </c>
       <c r="K21" t="n">
-        <v>0.00000000000000000000000000000000756075324165746</v>
+        <v>0.0000000000187644204456692</v>
       </c>
       <c r="L21" t="n">
-        <v>0.705547184026248</v>
+        <v>0.436890072574578</v>
       </c>
       <c r="M21" t="n">
-        <v>116.849980091699</v>
+        <v>9.00064914994108</v>
       </c>
       <c r="N21" t="n">
-        <v>0.000000000000000000263045248275305</v>
+        <v>0.00360948366546241</v>
       </c>
       <c r="O21" t="n">
-        <v>0.499679238997065</v>
+        <v>0.102279349492129</v>
       </c>
       <c r="P21" t="n">
-        <v>2.08489603304106</v>
+        <v>0.691795713820802</v>
       </c>
       <c r="Q21" t="n">
-        <v>760.312033864242</v>
+        <v>84.3713569008282</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" t="n">
-        <v>0.151535266640384</v>
+        <v>0.145482311989552</v>
       </c>
       <c r="D22" t="n">
-        <v>20.8961262617504</v>
+        <v>19.9193425034983</v>
       </c>
       <c r="E22" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F22" t="n">
-        <v>1037</v>
+        <v>62</v>
       </c>
       <c r="G22" t="n">
-        <v>206.100407674516</v>
+        <v>304.782972810231</v>
       </c>
       <c r="H22" t="n">
-        <v>0.00000000000000000000000000142931912179297</v>
+        <v>0.000000000000000000000000000000000227636619851689</v>
       </c>
       <c r="I22" t="n">
-        <v>0.637883465260549</v>
+        <v>0.722606156383082</v>
       </c>
       <c r="J22" t="n">
-        <v>217.521471940572</v>
+        <v>272.599588302447</v>
       </c>
       <c r="K22" t="n">
-        <v>0.000000000000000000000000000185569819894528</v>
+        <v>0.0000000000000000000000000000000240217325305129</v>
       </c>
       <c r="L22" t="n">
-        <v>0.650246666316281</v>
+        <v>0.699691674445065</v>
       </c>
       <c r="M22" t="n">
-        <v>56.8613005966153</v>
+        <v>72.673855636032</v>
       </c>
       <c r="N22" t="n">
-        <v>0.0000000000109496276810467</v>
+        <v>0.0000000000000623702300190497</v>
       </c>
       <c r="O22" t="n">
-        <v>0.327049782795208</v>
+        <v>0.383151675766464</v>
       </c>
       <c r="P22" t="n">
-        <v>1.76671518101242</v>
+        <v>0.990656298424169</v>
       </c>
       <c r="Q22" t="n">
-        <v>501.379306473454</v>
+        <v>312.438273309444</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
         <v>56</v>
       </c>
       <c r="C23" t="n">
-        <v>0.144708966161322</v>
+        <v>0.327634978393304</v>
       </c>
       <c r="D23" t="n">
-        <v>19.7955413666457</v>
+        <v>57.0126214781588</v>
       </c>
       <c r="E23" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F23" t="n">
-        <v>1100</v>
+        <v>121</v>
       </c>
       <c r="G23" t="n">
-        <v>414.388266020319</v>
+        <v>232.032520740648</v>
       </c>
       <c r="H23" t="n">
-        <v>0.000000000000000000000000000000000000000296599325392032</v>
+        <v>0.0000000000000000000000000000153099685903205</v>
       </c>
       <c r="I23" t="n">
-        <v>0.779822010605845</v>
+        <v>0.664787682959383</v>
       </c>
       <c r="J23" t="n">
-        <v>309.531531763336</v>
+        <v>212.904612487499</v>
       </c>
       <c r="K23" t="n">
-        <v>0.000000000000000000000000000000000118006100546677</v>
+        <v>0.000000000000000000000000000419942374723911</v>
       </c>
       <c r="L23" t="n">
-        <v>0.725694371254789</v>
+        <v>0.645352033371667</v>
       </c>
       <c r="M23" t="n">
-        <v>150.314659930915</v>
+        <v>70.2754463233988</v>
       </c>
       <c r="N23" t="n">
-        <v>0.0000000000000000000000993513674582184</v>
+        <v>0.000000000000132623686704838</v>
       </c>
       <c r="O23" t="n">
-        <v>0.562313566976696</v>
+        <v>0.375251789292457</v>
       </c>
       <c r="P23" t="n">
-        <v>2.21253891499865</v>
+        <v>1.30062199015827</v>
       </c>
       <c r="Q23" t="n">
-        <v>894.029999081216</v>
+        <v>326.929855443817</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>57</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0655955812130484</v>
+        <v>0.563278383777349</v>
       </c>
       <c r="D24" t="n">
-        <v>8.21344896023712</v>
+        <v>150.905218459236</v>
       </c>
       <c r="E24" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F24" t="n">
-        <v>1169</v>
+        <v>156</v>
       </c>
       <c r="G24" t="n">
-        <v>160.548164947788</v>
+        <v>46.9499952733394</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0000000000000000000000108828762396561</v>
+        <v>0.000000000361446274180731</v>
       </c>
       <c r="I24" t="n">
-        <v>0.578451545438935</v>
+        <v>0.28636777448553</v>
       </c>
       <c r="J24" t="n">
-        <v>139.73735940579</v>
+        <v>305.545214177662</v>
       </c>
       <c r="K24" t="n">
-        <v>0.00000000000000000000107093976248089</v>
+        <v>0.000000000000000000000000000000000204749496689107</v>
       </c>
       <c r="L24" t="n">
-        <v>0.544281361034512</v>
+        <v>0.723106555051865</v>
       </c>
       <c r="M24" t="n">
-        <v>42.1036792835897</v>
+        <v>21.5875299964547</v>
       </c>
       <c r="N24" t="n">
-        <v>0.00000000217051110198853</v>
+        <v>0.00000892785127956958</v>
       </c>
       <c r="O24" t="n">
-        <v>0.264630456524787</v>
+        <v>0.155768199325054</v>
       </c>
       <c r="P24" t="n">
-        <v>1.45295894421128</v>
+        <v>1.84966332260656</v>
       </c>
       <c r="Q24" t="n">
-        <v>350.602652597405</v>
+        <v>607.355651096134</v>
       </c>
     </row>
     <row r="25">
@@ -1905,49 +1884,49 @@
         <v>59</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0929904090914882</v>
+        <v>0.0290867179488445</v>
       </c>
       <c r="D25" t="n">
-        <v>11.9953283545836</v>
+        <v>2.51648046521852</v>
       </c>
       <c r="E25" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F25" t="n">
-        <v>1200</v>
+        <v>255</v>
       </c>
       <c r="G25" t="n">
-        <v>115.815108429033</v>
+        <v>92.8174314755556</v>
       </c>
       <c r="H25" t="n">
-        <v>0.000000000000000000341703215628054</v>
+        <v>0.00000000000000314538476275146</v>
       </c>
       <c r="I25" t="n">
-        <v>0.497455294935622</v>
+        <v>0.524933716664623</v>
       </c>
       <c r="J25" t="n">
-        <v>108.591525195017</v>
+        <v>84.3080072826521</v>
       </c>
       <c r="K25" t="n">
-        <v>0.00000000000000000219444354682105</v>
+        <v>0.0000000000000255304414025075</v>
       </c>
       <c r="L25" t="n">
-        <v>0.481363495819017</v>
+        <v>0.500915010781795</v>
       </c>
       <c r="M25" t="n">
-        <v>37.3063951267717</v>
+        <v>61.8059092309326</v>
       </c>
       <c r="N25" t="n">
-        <v>0.0000000135783567658168</v>
+        <v>0.0000000000114666857531666</v>
       </c>
       <c r="O25" t="n">
-        <v>0.241768301930211</v>
+        <v>0.423891662257956</v>
       </c>
       <c r="P25" t="n">
-        <v>1.31357750177634</v>
+        <v>0.559088446679484</v>
       </c>
       <c r="Q25" t="n">
-        <v>273.708357105405</v>
+        <v>89.3409682130891</v>
       </c>
     </row>
     <row r="26">
@@ -1958,102 +1937,102 @@
         <v>61</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0449779328522074</v>
+        <v>0.109032196399884</v>
       </c>
       <c r="D26" t="n">
-        <v>3.72060166728536</v>
+        <v>14.3178765015305</v>
       </c>
       <c r="E26" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F26" t="n">
-        <v>1272</v>
+        <v>287</v>
       </c>
       <c r="G26" t="n">
-        <v>77.2612979749472</v>
+        <v>158.955934598244</v>
       </c>
       <c r="H26" t="n">
-        <v>0.000000000000250329576138849</v>
+        <v>0.000000000000000000000015268704695483</v>
       </c>
       <c r="I26" t="n">
-        <v>0.494436555796011</v>
+        <v>0.576019264922363</v>
       </c>
       <c r="J26" t="n">
-        <v>77.6520716681098</v>
+        <v>145.551751964778</v>
       </c>
       <c r="K26" t="n">
-        <v>0.00000000000022653681163088</v>
+        <v>0.000000000000000000000286372554604455</v>
       </c>
       <c r="L26" t="n">
-        <v>0.495697700268064</v>
+        <v>0.55437356968886</v>
       </c>
       <c r="M26" t="n">
-        <v>22.7871549688665</v>
+        <v>11.5188815593455</v>
       </c>
       <c r="N26" t="n">
-        <v>0.00000816939091789053</v>
+        <v>0.000941081840897866</v>
       </c>
       <c r="O26" t="n">
-        <v>0.223870634520008</v>
+        <v>0.0896279318617202</v>
       </c>
       <c r="P26" t="n">
-        <v>1.25898282343629</v>
+        <v>0.772437962488628</v>
       </c>
       <c r="Q26" t="n">
-        <v>181.421126279209</v>
+        <v>174.187504967839</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
         <v>62</v>
       </c>
       <c r="C27" t="n">
-        <v>0.282629741542959</v>
+        <v>0.142002509453001</v>
       </c>
       <c r="D27" t="n">
-        <v>45.7017134910208</v>
+        <v>19.3640351971298</v>
       </c>
       <c r="E27" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F27" t="n">
-        <v>1294</v>
+        <v>326</v>
       </c>
       <c r="G27" t="n">
-        <v>184.405915173408</v>
+        <v>365.4812715123</v>
       </c>
       <c r="H27" t="n">
-        <v>0.000000000000000000000000100908504146196</v>
+        <v>0.000000000000000000000000000000000000085375277093501</v>
       </c>
       <c r="I27" t="n">
-        <v>0.613855805958283</v>
+        <v>0.757503540742063</v>
       </c>
       <c r="J27" t="n">
-        <v>207.683602835371</v>
+        <v>341.927445722141</v>
       </c>
       <c r="K27" t="n">
-        <v>0.00000000000000000000000000130216128019017</v>
+        <v>0.00000000000000000000000000000000000160853747871818</v>
       </c>
       <c r="L27" t="n">
-        <v>0.641625343440709</v>
+        <v>0.745057740410588</v>
       </c>
       <c r="M27" t="n">
-        <v>30.5633626362394</v>
+        <v>157.004637652616</v>
       </c>
       <c r="N27" t="n">
-        <v>0.000000201961636451644</v>
+        <v>0.0000000000000000000000231845010701126</v>
       </c>
       <c r="O27" t="n">
-        <v>0.208533443054904</v>
+        <v>0.572999928021901</v>
       </c>
       <c r="P27" t="n">
-        <v>1.74664433399685</v>
+        <v>1.02906275931659</v>
       </c>
       <c r="Q27" t="n">
-        <v>468.354594136039</v>
+        <v>380.655516116401</v>
       </c>
     </row>
     <row r="28">
@@ -2064,49 +2043,49 @@
         <v>64</v>
       </c>
       <c r="C28" t="n">
-        <v>0.271028897116847</v>
+        <v>0.12275312719125</v>
       </c>
       <c r="D28" t="n">
-        <v>41.6412068421216</v>
+        <v>16.3718063028163</v>
       </c>
       <c r="E28" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F28" t="n">
-        <v>1357</v>
+        <v>389</v>
       </c>
       <c r="G28" t="n">
-        <v>183.164990575492</v>
+        <v>124.693558089909</v>
       </c>
       <c r="H28" t="n">
-        <v>0.000000000000000000000000257188290252062</v>
+        <v>0.0000000000000000000375954381500522</v>
       </c>
       <c r="I28" t="n">
-        <v>0.620551205000192</v>
+        <v>0.51591593534952</v>
       </c>
       <c r="J28" t="n">
-        <v>130.261934593393</v>
+        <v>157.003551010054</v>
       </c>
       <c r="K28" t="n">
-        <v>0.000000000000000000017543551754832</v>
+        <v>0.0000000000000000000000231899137591237</v>
       </c>
       <c r="L28" t="n">
-        <v>0.537690474617985</v>
+        <v>0.572998234626139</v>
       </c>
       <c r="M28" t="n">
-        <v>56.8372047791921</v>
+        <v>21.6681061793255</v>
       </c>
       <c r="N28" t="n">
-        <v>0.0000000000132910520990479</v>
+        <v>0.00000861703801926928</v>
       </c>
       <c r="O28" t="n">
-        <v>0.336639100685922</v>
+        <v>0.156258758962961</v>
       </c>
       <c r="P28" t="n">
-        <v>1.76590967742095</v>
+        <v>0.818504489008639</v>
       </c>
       <c r="Q28" t="n">
-        <v>411.905336790199</v>
+        <v>189.747163615687</v>
       </c>
     </row>
     <row r="29">
@@ -2117,950 +2096,950 @@
         <v>66</v>
       </c>
       <c r="C29" t="n">
-        <v>0.283220540479796</v>
+        <v>0.378332061913549</v>
       </c>
       <c r="D29" t="n">
-        <v>44.2544775975727</v>
+        <v>71.2033684415772</v>
       </c>
       <c r="E29" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F29" t="n">
-        <v>1405</v>
+        <v>421</v>
       </c>
       <c r="G29" t="n">
-        <v>182.399184678458</v>
+        <v>131.227258167966</v>
       </c>
       <c r="H29" t="n">
-        <v>0.000000000000000000000000297693165784773</v>
+        <v>0.00000000000000000000780395258643625</v>
       </c>
       <c r="I29" t="n">
-        <v>0.619564163799142</v>
+        <v>0.528657727344229</v>
       </c>
       <c r="J29" t="n">
-        <v>131.716469793387</v>
+        <v>355.395758574116</v>
       </c>
       <c r="K29" t="n">
-        <v>0.0000000000000000000125157800951256</v>
+        <v>0.000000000000000000000000000000000000294778042628186</v>
       </c>
       <c r="L29" t="n">
-        <v>0.540449604842261</v>
+        <v>0.752326311410683</v>
       </c>
       <c r="M29" t="n">
-        <v>51.6727502440503</v>
+        <v>13.380763461592</v>
       </c>
       <c r="N29" t="n">
-        <v>0.0000000000780453989643719</v>
+        <v>0.000382493939664792</v>
       </c>
       <c r="O29" t="n">
-        <v>0.31570771656859</v>
+        <v>0.102628356410367</v>
       </c>
       <c r="P29" t="n">
-        <v>1.75894202568979</v>
+        <v>1.50899043523778</v>
       </c>
       <c r="Q29" t="n">
-        <v>410.042882313468</v>
+        <v>497.80249545727</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
         <v>67</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0870689118203738</v>
+        <v>0.250660845384867</v>
       </c>
       <c r="D30" t="n">
-        <v>11.1586326885818</v>
+        <v>39.1375770629418</v>
       </c>
       <c r="E30" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F30" t="n">
-        <v>1449</v>
+        <v>616</v>
       </c>
       <c r="G30" t="n">
-        <v>112.484924818282</v>
+        <v>209.935973035265</v>
       </c>
       <c r="H30" t="n">
-        <v>0.000000000000000000799439566637908</v>
+        <v>0.000000000000000000000000000714332529401071</v>
       </c>
       <c r="I30" t="n">
-        <v>0.490162588707529</v>
+        <v>0.642131763862585</v>
       </c>
       <c r="J30" t="n">
-        <v>101.209356207044</v>
+        <v>330.191372592944</v>
       </c>
       <c r="K30" t="n">
-        <v>0.0000000000000000156460076961204</v>
+        <v>0.00000000000000000000000000000000000735372175816255</v>
       </c>
       <c r="L30" t="n">
-        <v>0.46381767476099</v>
+        <v>0.738367045585874</v>
       </c>
       <c r="M30" t="n">
-        <v>46.3937833312236</v>
+        <v>21.717048889258</v>
       </c>
       <c r="N30" t="n">
-        <v>0.000000000442724389024693</v>
+        <v>0.00000843365913496514</v>
       </c>
       <c r="O30" t="n">
-        <v>0.283938485206482</v>
+        <v>0.156556451158324</v>
       </c>
       <c r="P30" t="n">
-        <v>1.32498766049537</v>
+        <v>1.23968873635561</v>
       </c>
       <c r="Q30" t="n">
-        <v>271.246697045131</v>
+        <v>408.466526718828</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
         <v>68</v>
       </c>
-      <c r="B31" t="s">
-        <v>69</v>
-      </c>
       <c r="C31" t="n">
-        <v>0.120973646701733</v>
+        <v>0.262867377187493</v>
       </c>
       <c r="D31" t="n">
-        <v>14.5879659947267</v>
+        <v>41.36652592773</v>
       </c>
       <c r="E31" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F31" t="n">
-        <v>1518</v>
+        <v>783</v>
       </c>
       <c r="G31" t="n">
-        <v>158.064921747329</v>
+        <v>292.597991858685</v>
       </c>
       <c r="H31" t="n">
-        <v>0.0000000000000000000000971821745704734</v>
+        <v>0.00000000000000000000000000000000167194663210551</v>
       </c>
       <c r="I31" t="n">
-        <v>0.598583563092768</v>
+        <v>0.716102373699088</v>
       </c>
       <c r="J31" t="n">
-        <v>143.832918604831</v>
+        <v>288.262613659115</v>
       </c>
       <c r="K31" t="n">
-        <v>0.00000000000000000000186647315743176</v>
+        <v>0.000000000000000000000000000000003110424140632</v>
       </c>
       <c r="L31" t="n">
-        <v>0.575716440443688</v>
+        <v>0.713057809254124</v>
       </c>
       <c r="M31" t="n">
-        <v>49.046251556681</v>
+        <v>102.147690838033</v>
       </c>
       <c r="N31" t="n">
-        <v>0.000000000238041625182797</v>
+        <v>0.0000000000000000131970929222747</v>
       </c>
       <c r="O31" t="n">
-        <v>0.316333036524594</v>
+        <v>0.468250158622463</v>
       </c>
       <c r="P31" t="n">
-        <v>1.61160668676278</v>
+        <v>1.23879256362911</v>
       </c>
       <c r="Q31" t="n">
-        <v>365.532057903568</v>
+        <v>370.995665514575</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0733653767474068</v>
+        <v>0.437122038368199</v>
       </c>
       <c r="D32" t="n">
-        <v>9.26335889470291</v>
+        <v>90.8603320350532</v>
       </c>
       <c r="E32" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F32" t="n">
-        <v>1576</v>
+        <v>826</v>
       </c>
       <c r="G32" t="n">
-        <v>191.608153469945</v>
+        <v>151.784624307862</v>
       </c>
       <c r="H32" t="n">
-        <v>0.0000000000000000000000000212204696027199</v>
+        <v>0.0000000000000000000000719369309619045</v>
       </c>
       <c r="I32" t="n">
-        <v>0.620878454815697</v>
+        <v>0.564707243573614</v>
       </c>
       <c r="J32" t="n">
-        <v>161.237997883998</v>
+        <v>248.990412480724</v>
       </c>
       <c r="K32" t="n">
-        <v>0.0000000000000000000000094036209523332</v>
+        <v>0.000000000000000000000000000000943537224952404</v>
       </c>
       <c r="L32" t="n">
-        <v>0.57949668668627</v>
+        <v>0.680319494691238</v>
       </c>
       <c r="M32" t="n">
-        <v>99.393592636415</v>
+        <v>37.7948331543923</v>
       </c>
       <c r="N32" t="n">
-        <v>0.0000000000000000256295729265239</v>
+        <v>0.0000000112343367324511</v>
       </c>
       <c r="O32" t="n">
-        <v>0.45931855664237</v>
+        <v>0.244160818447317</v>
       </c>
       <c r="P32" t="n">
-        <v>1.73305907489174</v>
+        <v>1.55456357142764</v>
       </c>
       <c r="Q32" t="n">
-        <v>461.503102885061</v>
+        <v>430.71107655083</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C33" t="n">
-        <v>0.474619306885485</v>
+        <v>0.363586208362164</v>
       </c>
       <c r="D33" t="n">
-        <v>97.5652242562702</v>
+        <v>55.4165586518272</v>
       </c>
       <c r="E33" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F33" t="n">
-        <v>1589</v>
+        <v>886</v>
       </c>
       <c r="G33" t="n">
-        <v>56.2363174287013</v>
+        <v>19.9043407208609</v>
       </c>
       <c r="H33" t="n">
-        <v>0.0000000000190200943225607</v>
+        <v>0.0000219408800900695</v>
       </c>
       <c r="I33" t="n">
-        <v>0.342410974071644</v>
+        <v>0.170261776407324</v>
       </c>
       <c r="J33" t="n">
-        <v>177.393561054351</v>
+        <v>48.0375856580225</v>
       </c>
       <c r="K33" t="n">
-        <v>0.00000000000000000000000157036885534887</v>
+        <v>0.000000000462968926239926</v>
       </c>
       <c r="L33" t="n">
-        <v>0.621575204426452</v>
+        <v>0.331207841333543</v>
       </c>
       <c r="M33" t="n">
-        <v>7.68755258160163</v>
+        <v>3.38059586340817</v>
       </c>
       <c r="N33" t="n">
-        <v>0.00655083242072182</v>
+        <v>0.0690279648861963</v>
       </c>
       <c r="O33" t="n">
-        <v>0.0664509915721409</v>
+        <v>0.0336777823874276</v>
       </c>
       <c r="P33" t="n">
-        <v>1.50505647695572</v>
+        <v>1.05838025805787</v>
       </c>
       <c r="Q33" t="n">
-        <v>338.882655320924</v>
+        <v>158.870702961677</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C34" t="n">
-        <v>0.0801273559325912</v>
+        <v>0.205442042695039</v>
       </c>
       <c r="D34" t="n">
-        <v>9.66887814946898</v>
+        <v>22.2362830921749</v>
       </c>
       <c r="E34" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F34" t="n">
-        <v>1678</v>
+        <v>949</v>
       </c>
       <c r="G34" t="n">
-        <v>132.176072558413</v>
+        <v>46.4483732775543</v>
       </c>
       <c r="H34" t="n">
-        <v>0.0000000000000000000127154668863986</v>
+        <v>0.00000000122372656110131</v>
       </c>
       <c r="I34" t="n">
-        <v>0.543540617166038</v>
+        <v>0.350690402064951</v>
       </c>
       <c r="J34" t="n">
-        <v>121.68553933979</v>
+        <v>67.3385270770083</v>
       </c>
       <c r="K34" t="n">
-        <v>0.000000000000000000149744382433354</v>
+        <v>0.00000000000202514511570712</v>
       </c>
       <c r="L34" t="n">
-        <v>0.522961330923507</v>
+        <v>0.439149432048413</v>
       </c>
       <c r="M34" t="n">
-        <v>34.985519331682</v>
+        <v>3.82688151055517</v>
       </c>
       <c r="N34" t="n">
-        <v>0.0000000374363501065221</v>
+        <v>0.0536821786327029</v>
       </c>
       <c r="O34" t="n">
-        <v>0.239650613922839</v>
+        <v>0.0426028539141202</v>
       </c>
       <c r="P34" t="n">
-        <v>1.38627991794498</v>
+        <v>0.850033517438491</v>
       </c>
       <c r="Q34" t="n">
-        <v>298.516009379354</v>
+        <v>111.811093261358</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C35" t="n">
-        <v>0.205359571421054</v>
+        <v>0.474619306885485</v>
       </c>
       <c r="D35" t="n">
-        <v>30.2364050357101</v>
+        <v>97.5652242562702</v>
       </c>
       <c r="E35" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F35" t="n">
-        <v>1698</v>
+        <v>1589</v>
       </c>
       <c r="G35" t="n">
-        <v>219.884547789505</v>
+        <v>56.2363174287013</v>
       </c>
       <c r="H35" t="n">
-        <v>0.000000000000000000000000000122707288102827</v>
+        <v>0.0000000000190200943225607</v>
       </c>
       <c r="I35" t="n">
-        <v>0.652700010232868</v>
+        <v>0.342410974071644</v>
       </c>
       <c r="J35" t="n">
-        <v>233.867272028628</v>
+        <v>177.393561054351</v>
       </c>
       <c r="K35" t="n">
-        <v>0.0000000000000000000000000000112515950928069</v>
+        <v>0.00000000000000000000000157036885534887</v>
       </c>
       <c r="L35" t="n">
-        <v>0.666540571528558</v>
+        <v>0.621575204426452</v>
       </c>
       <c r="M35" t="n">
-        <v>45.6646771123238</v>
+        <v>7.68755258160163</v>
       </c>
       <c r="N35" t="n">
-        <v>0.000000000578217806355115</v>
+        <v>0.00655083242072182</v>
       </c>
       <c r="O35" t="n">
-        <v>0.280728907609065</v>
+        <v>0.0664509915721409</v>
       </c>
       <c r="P35" t="n">
-        <v>1.80532906079155</v>
+        <v>1.57081381819742</v>
       </c>
       <c r="Q35" t="n">
-        <v>529.652901966167</v>
+        <v>372.524009566891</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C36" t="n">
-        <v>0.214413471217654</v>
+        <v>0.430679678511292</v>
       </c>
       <c r="D36" t="n">
-        <v>20.1971346106195</v>
+        <v>83.9693271263312</v>
       </c>
       <c r="E36" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F36" t="n">
-        <v>1765</v>
+        <v>1635</v>
       </c>
       <c r="G36" t="n">
-        <v>23.9461090679212</v>
+        <v>40.7203634461463</v>
       </c>
       <c r="H36" t="n">
-        <v>0.00000563117165089541</v>
+        <v>0.00000000418299893295757</v>
       </c>
       <c r="I36" t="n">
-        <v>0.244482494463518</v>
+        <v>0.268390890459475</v>
       </c>
       <c r="J36" t="n">
-        <v>36.4802427047669</v>
+        <v>23.5647417247755</v>
       </c>
       <c r="K36" t="n">
-        <v>0.0000000569628205065723</v>
+        <v>0.00000397950377468717</v>
       </c>
       <c r="L36" t="n">
-        <v>0.33019698193687</v>
+        <v>0.175118247341286</v>
       </c>
       <c r="M36" t="n">
-        <v>4.9433410474517</v>
+        <v>24.7040838192501</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0292441404378074</v>
+        <v>0.0000024484440880469</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0626188476679792</v>
+        <v>0.182043775868636</v>
       </c>
       <c r="P36" t="n">
-        <v>0.851711795286021</v>
+        <v>1.03647760436387</v>
       </c>
       <c r="Q36" t="n">
-        <v>85.5668274307593</v>
+        <v>191.503395977438</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0678043109289869</v>
+        <v>0.278980194964976</v>
       </c>
       <c r="D37" t="n">
-        <v>7.92823864978909</v>
+        <v>45.2701612118916</v>
       </c>
       <c r="E37" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F37" t="n">
-        <v>1822</v>
+        <v>1686</v>
       </c>
       <c r="G37" t="n">
-        <v>121.291500216623</v>
+        <v>169.734271979187</v>
       </c>
       <c r="H37" t="n">
-        <v>0.000000000000000000205875019890743</v>
+        <v>0.00000000000000000000000160180370137498</v>
       </c>
       <c r="I37" t="n">
-        <v>0.526686829963461</v>
+        <v>0.591956694983107</v>
       </c>
       <c r="J37" t="n">
-        <v>74.2650976905485</v>
+        <v>252.528392205882</v>
       </c>
       <c r="K37" t="n">
-        <v>0.0000000000000595261596159561</v>
+        <v>0.000000000000000000000000000000536276549405236</v>
       </c>
       <c r="L37" t="n">
-        <v>0.405233176564523</v>
+        <v>0.683380215247943</v>
       </c>
       <c r="M37" t="n">
-        <v>66.1601822325873</v>
+        <v>11.2805443654561</v>
       </c>
       <c r="N37" t="n">
-        <v>0.000000000000724333615913293</v>
+        <v>0.00105767732754649</v>
       </c>
       <c r="O37" t="n">
-        <v>0.377712453762672</v>
+        <v>0.0879365177412964</v>
       </c>
       <c r="P37" t="n">
-        <v>1.37743677121964</v>
+        <v>1.2413406051779</v>
       </c>
       <c r="Q37" t="n">
-        <v>269.645018789548</v>
+        <v>343.068714629665</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C38" t="n">
-        <v>0.0736732241467798</v>
+        <v>0.357314430430993</v>
       </c>
       <c r="D38" t="n">
-        <v>7.95326509685752</v>
+        <v>41.1418415223254</v>
       </c>
       <c r="E38" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F38" t="n">
-        <v>1877</v>
+        <v>1736</v>
       </c>
       <c r="G38" t="n">
-        <v>101.406391053381</v>
+        <v>0.0010895703698966</v>
       </c>
       <c r="H38" t="n">
-        <v>0.0000000000000000695171679767144</v>
+        <v>0.973756569059775</v>
       </c>
       <c r="I38" t="n">
-        <v>0.503491426081429</v>
+        <v>0.0000147237071267785</v>
       </c>
       <c r="J38" t="n">
-        <v>93.8727128912269</v>
+        <v>7.78239504993627</v>
       </c>
       <c r="K38" t="n">
-        <v>0.000000000000000476522347216398</v>
+        <v>0.00670493544741515</v>
       </c>
       <c r="L38" t="n">
-        <v>0.484197654694678</v>
+        <v>0.0951597840242311</v>
       </c>
       <c r="M38" t="n">
-        <v>32.4941687518172</v>
+        <v>0.289223283455362</v>
       </c>
       <c r="N38" t="n">
-        <v>0.00000012132736582059</v>
+        <v>0.592332454567753</v>
       </c>
       <c r="O38" t="n">
-        <v>0.245249802749311</v>
+        <v>0.00389320645272886</v>
       </c>
       <c r="P38" t="n">
-        <v>1.3066121076722</v>
+        <v>0.809788644886217</v>
       </c>
       <c r="Q38" t="n">
-        <v>235.726537793283</v>
+        <v>90.0660780945871</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C39" t="n">
-        <v>0.0963277142502427</v>
+        <v>0.148264984287294</v>
       </c>
       <c r="D39" t="n">
-        <v>11.0859682652694</v>
+        <v>18.9740740831139</v>
       </c>
       <c r="E39" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F39" t="n">
-        <v>1924</v>
+        <v>1803</v>
       </c>
       <c r="G39" t="n">
-        <v>172.91434813688</v>
+        <v>76.8232737471303</v>
       </c>
       <c r="H39" t="n">
-        <v>0.00000000000000000000000751580469392282</v>
+        <v>0.0000000000000276971645259865</v>
       </c>
       <c r="I39" t="n">
-        <v>0.624432606328538</v>
+        <v>0.413421161935141</v>
       </c>
       <c r="J39" t="n">
-        <v>155.368852349202</v>
+        <v>75.2069062496428</v>
       </c>
       <c r="K39" t="n">
-        <v>0.000000000000000000000230654513747978</v>
+        <v>0.0000000000000448566851015853</v>
       </c>
       <c r="L39" t="n">
-        <v>0.599026640793477</v>
+        <v>0.4082740858137</v>
       </c>
       <c r="M39" t="n">
-        <v>63.7289069407475</v>
+        <v>13.6302940691237</v>
       </c>
       <c r="N39" t="n">
-        <v>0.00000000000200533047246169</v>
+        <v>0.00034943636571943</v>
       </c>
       <c r="O39" t="n">
-        <v>0.379951840759689</v>
+        <v>0.111149485309401</v>
       </c>
       <c r="P39" t="n">
-        <v>1.69973880213195</v>
+        <v>0.704804054388288</v>
       </c>
       <c r="Q39" t="n">
-        <v>403.098075692099</v>
+        <v>113.155054415871</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C40" t="n">
-        <v>0.0848778286501301</v>
+        <v>0.422166622045089</v>
       </c>
       <c r="D40" t="n">
-        <v>10.8517816123029</v>
+        <v>84.7499123891934</v>
       </c>
       <c r="E40" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F40" t="n">
-        <v>1978</v>
+        <v>1286</v>
       </c>
       <c r="G40" t="n">
-        <v>197.999251818081</v>
+        <v>92.0251537636437</v>
       </c>
       <c r="H40" t="n">
-        <v>0.0000000000000000000000000063588283082778</v>
+        <v>0.000000000000000213402780884283</v>
       </c>
       <c r="I40" t="n">
-        <v>0.628570546359361</v>
+        <v>0.442375126751267</v>
       </c>
       <c r="J40" t="n">
-        <v>186.359716136638</v>
+        <v>179.563984878988</v>
       </c>
       <c r="K40" t="n">
-        <v>0.0000000000000000000000000581828480627772</v>
+        <v>0.000000000000000000000000260267730328162</v>
       </c>
       <c r="L40" t="n">
-        <v>0.614319259359733</v>
+        <v>0.607529990342045</v>
       </c>
       <c r="M40" t="n">
-        <v>90.1797472426351</v>
+        <v>9.85020291020907</v>
       </c>
       <c r="N40" t="n">
-        <v>0.000000000000000335335612096496</v>
+        <v>0.00215351121239125</v>
       </c>
       <c r="O40" t="n">
-        <v>0.435272986104296</v>
+        <v>0.0782692652250782</v>
       </c>
       <c r="P40" t="n">
-        <v>1.76304062047352</v>
+        <v>1.45186323443222</v>
       </c>
       <c r="Q40" t="n">
-        <v>485.390496809657</v>
+        <v>349.063809657375</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C41" t="n">
-        <v>0.13987803233348</v>
+        <v>0.57682150109473</v>
       </c>
       <c r="D41" t="n">
-        <v>15.9373294532523</v>
+        <v>152.663730056549</v>
       </c>
       <c r="E41" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F41" t="n">
-        <v>2000</v>
+        <v>1384</v>
       </c>
       <c r="G41" t="n">
-        <v>119.879186780643</v>
+        <v>46.6601743700054</v>
       </c>
       <c r="H41" t="n">
-        <v>0.00000000000000000106900378738976</v>
+        <v>0.000000000460694940642963</v>
       </c>
       <c r="I41" t="n">
-        <v>0.550209446583511</v>
+        <v>0.294088762698514</v>
       </c>
       <c r="J41" t="n">
-        <v>115.945479786196</v>
+        <v>61.5598329923247</v>
       </c>
       <c r="K41" t="n">
-        <v>0.00000000000000000262948665810407</v>
+        <v>0.00000000000276574085013894</v>
       </c>
       <c r="L41" t="n">
-        <v>0.541939375873073</v>
+        <v>0.354689399793598</v>
       </c>
       <c r="M41" t="n">
-        <v>32.8202241938052</v>
+        <v>25.5299812856638</v>
       </c>
       <c r="N41" t="n">
-        <v>0.000000111265244364946</v>
+        <v>0.00000170852769445215</v>
       </c>
       <c r="O41" t="n">
-        <v>0.250880354288212</v>
+        <v>0.185632114881449</v>
       </c>
       <c r="P41" t="n">
-        <v>1.48290720907828</v>
+        <v>1.50833240198306</v>
       </c>
       <c r="Q41" t="n">
-        <v>284.582220213897</v>
+        <v>366.887293105423</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C42" t="n">
-        <v>0.211418321157548</v>
+        <v>0.103148869263365</v>
       </c>
       <c r="D42" t="n">
-        <v>21.9841556049928</v>
+        <v>13.4564336155781</v>
       </c>
       <c r="E42" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F42" t="n">
-        <v>2065</v>
+        <v>1444</v>
       </c>
       <c r="G42" t="n">
-        <v>121.431504564428</v>
+        <v>113.852994341173</v>
       </c>
       <c r="H42" t="n">
-        <v>0.00000000000000000747391706041488</v>
+        <v>0.000000000000000000562970990822216</v>
       </c>
       <c r="I42" t="n">
-        <v>0.596915924229278</v>
+        <v>0.493183961793937</v>
       </c>
       <c r="J42" t="n">
-        <v>123.054109974567</v>
+        <v>105.491621665522</v>
       </c>
       <c r="K42" t="n">
-        <v>0.00000000000000000538238076258072</v>
+        <v>0.00000000000000000496628498696808</v>
       </c>
       <c r="L42" t="n">
-        <v>0.600105552577461</v>
+        <v>0.474137501789218</v>
       </c>
       <c r="M42" t="n">
-        <v>54.7106595600681</v>
+        <v>12.5889214146195</v>
       </c>
       <c r="N42" t="n">
-        <v>0.000000000108045465656653</v>
+        <v>0.000559512760368522</v>
       </c>
       <c r="O42" t="n">
-        <v>0.400193077380548</v>
+        <v>0.0971450435515342</v>
       </c>
       <c r="P42" t="n">
-        <v>1.80863287534484</v>
+        <v>0.680435240315948</v>
       </c>
       <c r="Q42" t="n">
-        <v>321.180429704056</v>
+        <v>132.404488896678</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C43" t="n">
-        <v>0.0862188310725256</v>
+        <v>0.508458653196011</v>
       </c>
       <c r="D43" t="n">
-        <v>8.96362195940594</v>
+        <v>109.648186442939</v>
       </c>
       <c r="E43" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F43" t="n">
-        <v>2125</v>
+        <v>1481</v>
       </c>
       <c r="G43" t="n">
-        <v>101.372891449438</v>
+        <v>2.84606920984938</v>
       </c>
       <c r="H43" t="n">
-        <v>0.000000000000000118008271140421</v>
+        <v>0.0945384504414863</v>
       </c>
       <c r="I43" t="n">
-        <v>0.516226505100575</v>
+        <v>0.0261476526484597</v>
       </c>
       <c r="J43" t="n">
-        <v>94.7485452980491</v>
+        <v>7.62761066224394</v>
       </c>
       <c r="K43" t="n">
-        <v>0.000000000000000612000629623154</v>
+        <v>0.00677675009818051</v>
       </c>
       <c r="L43" t="n">
-        <v>0.499337400185186</v>
+        <v>0.0671281444517643</v>
       </c>
       <c r="M43" t="n">
-        <v>34.0061537887678</v>
+        <v>0.116607812687753</v>
       </c>
       <c r="N43" t="n">
-        <v>0.0000000754411128612946</v>
+        <v>0.733419121215096</v>
       </c>
       <c r="O43" t="n">
-        <v>0.263601020494331</v>
+        <v>0.00109886487225056</v>
       </c>
       <c r="P43" t="n">
-        <v>1.36538375685262</v>
+        <v>1.08404545084379</v>
       </c>
       <c r="Q43" t="n">
-        <v>239.091212495661</v>
+        <v>226.923983548122</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C44" t="n">
-        <v>0.0910478569453192</v>
+        <v>0.214840281547653</v>
       </c>
       <c r="D44" t="n">
-        <v>11.6194801743502</v>
+        <v>31.4670146689136</v>
       </c>
       <c r="E44" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F44" t="n">
-        <v>2182</v>
+        <v>470</v>
       </c>
       <c r="G44" t="n">
-        <v>154.762310914605</v>
+        <v>202.925560409737</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0000000000000000000000432480692520867</v>
+        <v>0.00000000000000000000000000373658533410942</v>
       </c>
       <c r="I44" t="n">
-        <v>0.571579960267864</v>
+        <v>0.638280106035546</v>
       </c>
       <c r="J44" t="n">
-        <v>124.113572634054</v>
+        <v>148.971918312198</v>
       </c>
       <c r="K44" t="n">
-        <v>0.0000000000000000000482050496200292</v>
+        <v>0.000000000000000000000174827441857826</v>
       </c>
       <c r="L44" t="n">
-        <v>0.516895281147681</v>
+        <v>0.564347599035174</v>
       </c>
       <c r="M44" t="n">
-        <v>75.2126284125183</v>
+        <v>50.911989009451</v>
       </c>
       <c r="N44" t="n">
-        <v>0.0000000000000299560991182922</v>
+        <v>0.000000000092535780137685</v>
       </c>
       <c r="O44" t="n">
-        <v>0.393345507757239</v>
+        <v>0.306861422814664</v>
       </c>
       <c r="P44" t="n">
-        <v>1.5728686061181</v>
+        <v>0.99402816213048</v>
       </c>
       <c r="Q44" t="n">
-        <v>365.707992135527</v>
+        <v>211.905947650025</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C45" t="n">
-        <v>0.112317175750371</v>
+        <v>0.271982572653854</v>
       </c>
       <c r="D45" t="n">
-        <v>10.1222799569487</v>
+        <v>41.0952840799222</v>
       </c>
       <c r="E45" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F45" t="n">
-        <v>2213</v>
+        <v>523</v>
       </c>
       <c r="G45" t="n">
-        <v>73.4544256014574</v>
+        <v>113.351310246852</v>
       </c>
       <c r="H45" t="n">
-        <v>0.000000000000613548085044047</v>
+        <v>0.00000000000000000127667785162738</v>
       </c>
       <c r="I45" t="n">
-        <v>0.478672578607989</v>
+        <v>0.507502329498644</v>
       </c>
       <c r="J45" t="n">
-        <v>66.6856808403044</v>
+        <v>138.327672548179</v>
       </c>
       <c r="K45" t="n">
-        <v>0.00000000000382088576182923</v>
+        <v>0.00000000000000000000358508309513002</v>
       </c>
       <c r="L45" t="n">
-        <v>0.45461615924805</v>
+        <v>0.557036882473667</v>
       </c>
       <c r="M45" t="n">
-        <v>9.80965432924024</v>
+        <v>21.8697943772819</v>
       </c>
       <c r="N45" t="n">
-        <v>0.00242521529765545</v>
+        <v>0.00000834250428612088</v>
       </c>
       <c r="O45" t="n">
-        <v>0.109227169422992</v>
+        <v>0.165843849841094</v>
       </c>
       <c r="P45" t="n">
-        <v>1.1548330830294</v>
+        <v>1.10100202778138</v>
       </c>
       <c r="Q45" t="n">
-        <v>160.072040727951</v>
+        <v>220.518240708023</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C46" t="n">
-        <v>0.123200961856476</v>
+        <v>0.082738386327401</v>
       </c>
       <c r="D46" t="n">
-        <v>16.4399274065447</v>
+        <v>10.5535771431085</v>
       </c>
       <c r="E46" t="n">
         <v>0.000999000999000999</v>
       </c>
       <c r="F46" t="n">
-        <v>2277</v>
+        <v>586</v>
       </c>
       <c r="G46" t="n">
-        <v>400.077392634276</v>
+        <v>196.701876575762</v>
       </c>
       <c r="H46" t="n">
-        <v>0.00000000000000000000000000000000000000147040587009216</v>
+        <v>0.00000000000000000000000000810494846623105</v>
       </c>
       <c r="I46" t="n">
-        <v>0.773728262603132</v>
+        <v>0.627034427472596</v>
       </c>
       <c r="J46" t="n">
-        <v>317.327331500022</v>
+        <v>184.679848910188</v>
       </c>
       <c r="K46" t="n">
-        <v>0.0000000000000000000000000000000000407668864797863</v>
+        <v>0.00000000000000000000000008065181583648</v>
       </c>
       <c r="L46" t="n">
-        <v>0.730617919908653</v>
+        <v>0.612171643473506</v>
       </c>
       <c r="M46" t="n">
-        <v>139.05433535319</v>
+        <v>96.7005810640409</v>
       </c>
       <c r="N46" t="n">
-        <v>0.00000000000000000000125290128156216</v>
+        <v>0.0000000000000000537076490495902</v>
       </c>
       <c r="O46" t="n">
-        <v>0.543065733143649</v>
+        <v>0.452504998267001</v>
       </c>
       <c r="P46" t="n">
-        <v>2.17061287751191</v>
+        <v>0.777648416128308</v>
       </c>
       <c r="Q46" t="n">
-        <v>872.898986894033</v>
+        <v>205.787003196405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>